<commit_message>
go back to tomrw
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cinnamon\Documents\gamepithing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEEBFC2-5730-40B6-A2A8-453A8B5CBE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09826A31-6D4E-4D6A-97A5-D0161C40EDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19245" yWindow="5265" windowWidth="38700" windowHeight="15435" xr2:uid="{63D8B6F8-5ABE-4A23-BC17-1C5DB2606248}"/>
+    <workbookView xWindow="11370" yWindow="6315" windowWidth="38700" windowHeight="15435" xr2:uid="{63D8B6F8-5ABE-4A23-BC17-1C5DB2606248}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,10 +454,13 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>